<commit_message>
Template para primera prueba.
</commit_message>
<xml_diff>
--- a/Input_template.xlsx
+++ b/Input_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t xml:space="preserve">Etiqueta</t>
   </si>
@@ -116,19 +116,10 @@
     <t xml:space="preserve">fluorescence</t>
   </si>
   <si>
-    <t xml:space="preserve">v9_no_fl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versión 9 – sin fluorescencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, 0.1, 1.0, 5.0, 10.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, 0.004, 0.008, 0.012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01, 0.018, 0.03</t>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0, 1</t>
   </si>
   <si>
     <t xml:space="preserve">Voss92: 0.314</t>
@@ -390,10 +381,10 @@
   <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.33"/>
@@ -514,16 +505,16 @@
         <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>4500</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>6000</v>
+        <v>1</v>
       </c>
       <c r="F2" s="8" t="n">
         <v>0.5</v>
@@ -531,8 +522,8 @@
       <c r="G2" s="8" t="n">
         <v>100</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>1.5</v>
+      <c r="H2" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="I2" s="8" t="n">
         <v>10</v>
@@ -540,8 +531,8 @@
       <c r="J2" s="8" t="n">
         <v>500</v>
       </c>
-      <c r="K2" s="8" t="n">
-        <v>1.5</v>
+      <c r="K2" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="L2" s="8" t="n">
         <v>1</v>
@@ -550,7 +541,7 @@
         <v>10</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O2" s="8" t="n">
         <v>0.314</v>
@@ -561,8 +552,8 @@
       <c r="Q2" s="8" t="n">
         <v>0.041</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>34</v>
+      <c r="R2" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="S2" s="8" t="n">
         <v>0.55</v>
@@ -576,8 +567,8 @@
       <c r="V2" s="8" t="n">
         <v>-0.0149</v>
       </c>
-      <c r="W2" s="8" t="s">
-        <v>35</v>
+      <c r="W2" s="8" t="n">
+        <v>0.1</v>
       </c>
       <c r="X2" s="0" t="n">
         <v>0.006</v>
@@ -607,27 +598,27 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N3" s="8"/>
       <c r="O3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="AE3" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="AC3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE3" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O4" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -652,16 +643,16 @@
       <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>